<commit_message>
Added new non-bond template: NonBondPotential-LJ-AB
</commit_message>
<xml_diff>
--- a/XML/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
+++ b/XML/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Coarse-Grained\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\XML\Coarse-Grained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9CB7B593-33C2-4700-BC55-E84218F77A47}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F74F20CE-8116-4E35-83C0-3CC9C437CA1E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -28,17 +28,18 @@
     <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId13"/>
     <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId14"/>
     <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId15"/>
-    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId16"/>
-    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId17"/>
-    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId18"/>
-    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId19"/>
-    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId20"/>
-    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId21"/>
-    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId22"/>
-    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId23"/>
-    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId24"/>
-    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId25"/>
-    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId26"/>
+    <sheet name="NonBondPotential-LJ-AB" sheetId="56" r:id="rId16"/>
+    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId17"/>
+    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId18"/>
+    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId19"/>
+    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId20"/>
+    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId21"/>
+    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId22"/>
+    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId23"/>
+    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId24"/>
+    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId25"/>
+    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId26"/>
+    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="248">
   <si>
     <t>AT-1</t>
   </si>
@@ -787,12 +788,33 @@
   </si>
   <si>
     <t>Data Contact (Name)</t>
+  </si>
+  <si>
+    <t>A/(R^12)-B/(R^6)</t>
+  </si>
+  <si>
+    <t>A-units</t>
+  </si>
+  <si>
+    <t>B-units</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Lennard-Jones (12-6) [A-B Form]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1045,7 +1067,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1114,18 +1136,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1480,8 +1512,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,10 +1524,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="44"/>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -1518,10 +1550,10 @@
       <c r="B5" s="24"/>
     </row>
     <row r="6" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="B6" s="45"/>
+      <c r="B6" s="43"/>
     </row>
     <row r="7" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
@@ -1622,12 +1654,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1965,12 +1997,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2456,15 +2488,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2571,6 +2603,2931 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E701295-13E7-4A34-A798-03BF4464E0DA}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:G711"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" style="48" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+      <c r="F9" s="49"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="F10" s="49"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="F11" s="49"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="F12" s="49"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="F13" s="49"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="F14" s="49"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="F15" s="49"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="F16" s="49"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="F17" s="49"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="F18" s="49"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="F19" s="49"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="F20" s="49"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="F21" s="49"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="F22" s="49"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="F23" s="49"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="F24" s="49"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="F25" s="49"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="F26" s="49"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="F27" s="49"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28"/>
+      <c r="F28" s="49"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29"/>
+      <c r="F29" s="49"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30"/>
+      <c r="F30" s="49"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+      <c r="F31" s="49"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32"/>
+      <c r="F32" s="49"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33"/>
+      <c r="F33" s="49"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34"/>
+      <c r="F34" s="49"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35"/>
+      <c r="F35" s="49"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36"/>
+      <c r="F36" s="49"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37"/>
+      <c r="F37" s="49"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38"/>
+      <c r="F38" s="49"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39"/>
+      <c r="F39" s="49"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40"/>
+      <c r="F40" s="49"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41"/>
+      <c r="F41" s="49"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42"/>
+      <c r="F42" s="49"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="F43" s="49"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="F44" s="49"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="F45" s="49"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46"/>
+      <c r="F46" s="49"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47"/>
+      <c r="F47" s="49"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="F48" s="49"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49"/>
+      <c r="F49" s="49"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50"/>
+      <c r="F50" s="49"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51"/>
+      <c r="F51" s="49"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52"/>
+      <c r="F52" s="49"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53"/>
+      <c r="F53" s="49"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54"/>
+      <c r="F54" s="49"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55"/>
+      <c r="F55" s="49"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+      <c r="F56" s="49"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+      <c r="F57" s="49"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+      <c r="F58" s="49"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59"/>
+      <c r="F59" s="49"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60"/>
+      <c r="F60" s="49"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61"/>
+      <c r="F61" s="49"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62"/>
+      <c r="F62" s="49"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63"/>
+      <c r="F63" s="49"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64"/>
+      <c r="F64" s="49"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65"/>
+      <c r="F65" s="49"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66"/>
+      <c r="F66" s="49"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67"/>
+      <c r="F67" s="49"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68"/>
+      <c r="F68" s="49"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69"/>
+      <c r="F69" s="49"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70"/>
+      <c r="F70" s="49"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71"/>
+      <c r="F71" s="49"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72"/>
+      <c r="F72" s="49"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73"/>
+      <c r="F73" s="49"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74"/>
+      <c r="F74" s="49"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75"/>
+      <c r="F75" s="49"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76"/>
+      <c r="F76" s="49"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77"/>
+      <c r="F77" s="49"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78"/>
+      <c r="F78" s="49"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79"/>
+      <c r="F79" s="49"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80"/>
+      <c r="F80" s="49"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81"/>
+      <c r="F81" s="49"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82"/>
+      <c r="F82" s="49"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83"/>
+      <c r="F83" s="49"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84"/>
+      <c r="F84" s="49"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85"/>
+      <c r="F85" s="49"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86"/>
+      <c r="F86" s="49"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87"/>
+      <c r="F87" s="49"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88"/>
+      <c r="F88" s="49"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89"/>
+      <c r="F89" s="49"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90"/>
+      <c r="F90" s="49"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91"/>
+      <c r="F91" s="49"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92"/>
+      <c r="F92" s="49"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93"/>
+      <c r="F93" s="49"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94"/>
+      <c r="F94" s="49"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95"/>
+      <c r="F95" s="49"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96"/>
+      <c r="F96" s="49"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97"/>
+      <c r="F97" s="49"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98"/>
+      <c r="F98" s="49"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99"/>
+      <c r="F99" s="49"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100"/>
+      <c r="F100" s="49"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101"/>
+      <c r="F101" s="49"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102"/>
+      <c r="F102" s="49"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103"/>
+      <c r="F103" s="49"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104"/>
+      <c r="F104" s="49"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105"/>
+      <c r="F105" s="49"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106"/>
+      <c r="F106" s="49"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107"/>
+      <c r="F107" s="49"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108"/>
+      <c r="F108" s="49"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109"/>
+      <c r="F109" s="49"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110"/>
+      <c r="F110" s="49"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111"/>
+      <c r="F111" s="49"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112"/>
+      <c r="F112" s="49"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113"/>
+      <c r="F113" s="49"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114"/>
+      <c r="F114" s="49"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115"/>
+      <c r="F115" s="49"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116"/>
+      <c r="F116" s="49"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117"/>
+      <c r="F117" s="49"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118"/>
+      <c r="F118" s="49"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119"/>
+      <c r="F119" s="49"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120"/>
+      <c r="F120" s="49"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121"/>
+      <c r="F121" s="49"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122"/>
+      <c r="F122" s="49"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123"/>
+      <c r="F123" s="49"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124"/>
+      <c r="F124" s="49"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125"/>
+      <c r="F125" s="49"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126"/>
+      <c r="F126" s="49"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127"/>
+      <c r="F127" s="49"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128"/>
+      <c r="F128" s="49"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129"/>
+      <c r="F129" s="49"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130"/>
+      <c r="F130" s="49"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131"/>
+      <c r="F131" s="49"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132"/>
+      <c r="F132" s="49"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133"/>
+      <c r="F133" s="49"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134"/>
+      <c r="F134" s="49"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135"/>
+      <c r="F135" s="49"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136"/>
+      <c r="F136" s="49"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137"/>
+      <c r="F137" s="49"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138"/>
+      <c r="F138" s="49"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139"/>
+      <c r="F139" s="49"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140"/>
+      <c r="F140" s="49"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141"/>
+      <c r="F141" s="49"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142"/>
+      <c r="F142" s="49"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143"/>
+      <c r="F143" s="49"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144"/>
+      <c r="F144" s="49"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145"/>
+      <c r="F145" s="49"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146"/>
+      <c r="F146" s="49"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147"/>
+      <c r="F147" s="49"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148"/>
+      <c r="F148" s="49"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149"/>
+      <c r="F149" s="49"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150"/>
+      <c r="F150" s="49"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151"/>
+      <c r="F151" s="49"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152"/>
+      <c r="F152" s="49"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153"/>
+      <c r="F153" s="49"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154"/>
+      <c r="F154" s="49"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155"/>
+      <c r="F155" s="49"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156"/>
+      <c r="F156" s="49"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157"/>
+      <c r="F157" s="49"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158"/>
+      <c r="F158" s="49"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159"/>
+      <c r="F159" s="49"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160"/>
+      <c r="F160" s="49"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161"/>
+      <c r="F161" s="49"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162"/>
+      <c r="F162" s="49"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163"/>
+      <c r="F163" s="49"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164"/>
+      <c r="F164" s="49"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165"/>
+      <c r="F165" s="49"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166"/>
+      <c r="F166" s="49"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167"/>
+      <c r="F167" s="49"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168"/>
+      <c r="F168" s="49"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169"/>
+      <c r="F169" s="49"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170"/>
+      <c r="F170" s="49"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171"/>
+      <c r="F171" s="49"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172"/>
+      <c r="F172" s="49"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173"/>
+      <c r="F173" s="49"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174"/>
+      <c r="F174" s="49"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175"/>
+      <c r="F175" s="49"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176"/>
+      <c r="F176" s="49"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177"/>
+      <c r="F177" s="49"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178"/>
+      <c r="F178" s="49"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179"/>
+      <c r="F179" s="49"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180"/>
+      <c r="F180" s="49"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181"/>
+      <c r="F181" s="49"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182"/>
+      <c r="F182" s="49"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183"/>
+      <c r="F183" s="49"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184"/>
+      <c r="F184" s="49"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185"/>
+      <c r="F185" s="49"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186"/>
+      <c r="F186" s="49"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187"/>
+      <c r="F187" s="49"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188"/>
+      <c r="F188" s="49"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189"/>
+      <c r="F189" s="49"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190"/>
+      <c r="F190" s="49"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191"/>
+      <c r="F191" s="49"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192"/>
+      <c r="F192" s="49"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193"/>
+      <c r="F193" s="49"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194"/>
+      <c r="F194" s="49"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195"/>
+      <c r="F195" s="49"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196"/>
+      <c r="F196" s="49"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197"/>
+      <c r="F197" s="49"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198"/>
+      <c r="F198" s="49"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199"/>
+      <c r="F199" s="49"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200"/>
+      <c r="F200" s="49"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201"/>
+      <c r="F201" s="49"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202"/>
+      <c r="F202" s="49"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203"/>
+      <c r="F203" s="49"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204"/>
+      <c r="F204" s="49"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205"/>
+      <c r="F205" s="49"/>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206"/>
+      <c r="F206" s="49"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207"/>
+      <c r="F207" s="49"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208"/>
+      <c r="F208" s="49"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209"/>
+      <c r="F209" s="49"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210"/>
+      <c r="F210" s="49"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211"/>
+      <c r="F211" s="49"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212"/>
+      <c r="F212" s="49"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213"/>
+      <c r="F213" s="49"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214"/>
+      <c r="F214" s="49"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215"/>
+      <c r="F215" s="49"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216"/>
+      <c r="F216" s="49"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217"/>
+      <c r="F217" s="49"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218"/>
+      <c r="F218" s="49"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219"/>
+      <c r="F219" s="49"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220"/>
+      <c r="F220" s="49"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221"/>
+      <c r="F221" s="49"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222"/>
+      <c r="F222" s="49"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223"/>
+      <c r="F223" s="49"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224"/>
+      <c r="F224" s="49"/>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225"/>
+      <c r="F225" s="49"/>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226"/>
+      <c r="F226" s="49"/>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227"/>
+      <c r="F227" s="49"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228"/>
+      <c r="F228" s="49"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229"/>
+      <c r="F229" s="49"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230"/>
+      <c r="F230" s="49"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231"/>
+      <c r="F231" s="49"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232"/>
+      <c r="F232" s="49"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233"/>
+      <c r="F233" s="49"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234"/>
+      <c r="F234" s="49"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235"/>
+      <c r="F235" s="49"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236"/>
+      <c r="F236" s="49"/>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237"/>
+      <c r="F237" s="49"/>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238"/>
+      <c r="F238" s="49"/>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239"/>
+      <c r="F239" s="49"/>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240"/>
+      <c r="F240" s="49"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241"/>
+      <c r="F241" s="49"/>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242"/>
+      <c r="F242" s="49"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243"/>
+      <c r="F243" s="49"/>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244"/>
+      <c r="F244" s="49"/>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245"/>
+      <c r="F245" s="49"/>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246"/>
+      <c r="F246" s="49"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247"/>
+      <c r="F247" s="49"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248"/>
+      <c r="F248" s="49"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249"/>
+      <c r="F249" s="49"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250"/>
+      <c r="F250" s="49"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251"/>
+      <c r="F251" s="49"/>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252"/>
+      <c r="F252" s="49"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253"/>
+      <c r="F253" s="49"/>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254"/>
+      <c r="F254" s="49"/>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255"/>
+      <c r="F255" s="49"/>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256"/>
+      <c r="F256" s="49"/>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257"/>
+      <c r="F257" s="49"/>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258"/>
+      <c r="F258" s="49"/>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259"/>
+      <c r="F259" s="49"/>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260"/>
+      <c r="F260" s="49"/>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261"/>
+      <c r="F261" s="49"/>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262"/>
+      <c r="F262" s="49"/>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263"/>
+      <c r="F263" s="49"/>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264"/>
+      <c r="F264" s="49"/>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265"/>
+      <c r="F265" s="49"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266"/>
+      <c r="F266" s="49"/>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267"/>
+      <c r="F267" s="49"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268"/>
+      <c r="F268" s="49"/>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269"/>
+      <c r="F269" s="49"/>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270"/>
+      <c r="F270" s="49"/>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271"/>
+      <c r="F271" s="49"/>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272"/>
+      <c r="F272" s="49"/>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273"/>
+      <c r="F273" s="49"/>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274"/>
+      <c r="F274" s="49"/>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275"/>
+      <c r="F275" s="49"/>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276"/>
+      <c r="F276" s="49"/>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277"/>
+      <c r="F277" s="49"/>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278"/>
+      <c r="F278" s="49"/>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279"/>
+      <c r="F279" s="49"/>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280"/>
+      <c r="F280" s="49"/>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281"/>
+      <c r="F281" s="49"/>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282"/>
+      <c r="F282" s="49"/>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283"/>
+      <c r="F283" s="49"/>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284"/>
+      <c r="F284" s="49"/>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285"/>
+      <c r="F285" s="49"/>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286"/>
+      <c r="F286" s="49"/>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287"/>
+      <c r="F287" s="49"/>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288"/>
+      <c r="F288" s="49"/>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289"/>
+      <c r="F289" s="49"/>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290"/>
+      <c r="F290" s="49"/>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291"/>
+      <c r="F291" s="49"/>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292"/>
+      <c r="F292" s="49"/>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293"/>
+      <c r="F293" s="49"/>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294"/>
+      <c r="F294" s="49"/>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295"/>
+      <c r="F295" s="49"/>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296"/>
+      <c r="F296" s="49"/>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297"/>
+      <c r="F297" s="49"/>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298"/>
+      <c r="F298" s="49"/>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299"/>
+      <c r="F299" s="49"/>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300"/>
+      <c r="F300" s="49"/>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301"/>
+      <c r="F301" s="49"/>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302"/>
+      <c r="F302" s="49"/>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303"/>
+      <c r="F303" s="49"/>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304"/>
+      <c r="F304" s="49"/>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305"/>
+      <c r="F305" s="49"/>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306"/>
+      <c r="F306" s="49"/>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307"/>
+      <c r="F307" s="49"/>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308"/>
+      <c r="F308" s="49"/>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309"/>
+      <c r="F309" s="49"/>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310"/>
+      <c r="F310" s="49"/>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311"/>
+      <c r="F311" s="49"/>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312"/>
+      <c r="F312" s="49"/>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313"/>
+      <c r="F313" s="49"/>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314"/>
+      <c r="F314" s="49"/>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315"/>
+      <c r="F315" s="49"/>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316"/>
+      <c r="F316" s="49"/>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317"/>
+      <c r="F317" s="49"/>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318"/>
+      <c r="F318" s="49"/>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319"/>
+      <c r="F319" s="49"/>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320"/>
+      <c r="F320" s="49"/>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321"/>
+      <c r="F321" s="49"/>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322"/>
+      <c r="F322" s="49"/>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323"/>
+      <c r="F323" s="49"/>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324"/>
+      <c r="F324" s="49"/>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325"/>
+      <c r="F325" s="49"/>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326"/>
+      <c r="F326" s="49"/>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327"/>
+      <c r="F327" s="49"/>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328"/>
+      <c r="F328" s="49"/>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329"/>
+      <c r="F329" s="49"/>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330"/>
+      <c r="F330" s="49"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331"/>
+      <c r="F331" s="49"/>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332"/>
+      <c r="F332" s="49"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333"/>
+      <c r="F333" s="49"/>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334"/>
+      <c r="F334" s="49"/>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335"/>
+      <c r="F335" s="49"/>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336"/>
+      <c r="F336" s="49"/>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337"/>
+      <c r="F337" s="49"/>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338"/>
+      <c r="F338" s="49"/>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339"/>
+      <c r="F339" s="49"/>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340"/>
+      <c r="F340" s="49"/>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341"/>
+      <c r="F341" s="49"/>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342"/>
+      <c r="F342" s="49"/>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343"/>
+      <c r="F343" s="49"/>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344"/>
+      <c r="F344" s="49"/>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345"/>
+      <c r="F345" s="49"/>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346"/>
+      <c r="F346" s="49"/>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347"/>
+      <c r="F347" s="49"/>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348"/>
+      <c r="F348" s="49"/>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349"/>
+      <c r="F349" s="49"/>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350"/>
+      <c r="F350" s="49"/>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351"/>
+      <c r="F351" s="49"/>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352"/>
+      <c r="F352" s="49"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353"/>
+      <c r="F353" s="49"/>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354"/>
+      <c r="F354" s="49"/>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355"/>
+      <c r="F355" s="49"/>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356"/>
+      <c r="F356" s="49"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357"/>
+      <c r="F357" s="49"/>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358"/>
+      <c r="F358" s="49"/>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359"/>
+      <c r="F359" s="49"/>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360"/>
+      <c r="F360" s="49"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361"/>
+      <c r="F361" s="49"/>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362"/>
+      <c r="F362" s="49"/>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363"/>
+      <c r="F363" s="49"/>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364"/>
+      <c r="F364" s="49"/>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365"/>
+      <c r="F365" s="49"/>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366"/>
+      <c r="F366" s="49"/>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367"/>
+      <c r="F367" s="49"/>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368"/>
+      <c r="F368" s="49"/>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369"/>
+      <c r="F369" s="49"/>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370"/>
+      <c r="F370" s="49"/>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371"/>
+      <c r="F371" s="49"/>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372"/>
+      <c r="F372" s="49"/>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373"/>
+      <c r="F373" s="49"/>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374"/>
+      <c r="F374" s="49"/>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375"/>
+      <c r="F375" s="49"/>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376"/>
+      <c r="F376" s="49"/>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377"/>
+      <c r="F377" s="49"/>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378"/>
+      <c r="F378" s="49"/>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379"/>
+      <c r="F379" s="49"/>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380"/>
+      <c r="F380" s="49"/>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381"/>
+      <c r="F381" s="49"/>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382"/>
+      <c r="F382" s="49"/>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383"/>
+      <c r="F383" s="49"/>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384"/>
+      <c r="F384" s="49"/>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385"/>
+      <c r="F385" s="49"/>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386"/>
+      <c r="F386" s="49"/>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387"/>
+      <c r="F387" s="49"/>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388"/>
+      <c r="F388" s="49"/>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389"/>
+      <c r="F389" s="49"/>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390"/>
+      <c r="F390" s="49"/>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391"/>
+      <c r="F391" s="49"/>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392"/>
+      <c r="F392" s="49"/>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393"/>
+      <c r="F393" s="49"/>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394"/>
+      <c r="F394" s="49"/>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395"/>
+      <c r="F395" s="49"/>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396"/>
+      <c r="F396" s="49"/>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397"/>
+      <c r="F397" s="49"/>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398"/>
+      <c r="F398" s="49"/>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399"/>
+      <c r="F399" s="49"/>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A400"/>
+      <c r="F400" s="49"/>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A401"/>
+      <c r="F401" s="49"/>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A402"/>
+      <c r="F402" s="49"/>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A403"/>
+      <c r="F403" s="49"/>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A404"/>
+      <c r="F404" s="49"/>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A405"/>
+      <c r="F405" s="49"/>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A406"/>
+      <c r="F406" s="49"/>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A407"/>
+      <c r="F407" s="49"/>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A408"/>
+      <c r="F408" s="49"/>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A409"/>
+      <c r="F409" s="49"/>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A410"/>
+      <c r="F410" s="49"/>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A411"/>
+      <c r="F411" s="49"/>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A412"/>
+      <c r="F412" s="49"/>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A413"/>
+      <c r="F413" s="49"/>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A414"/>
+      <c r="F414" s="49"/>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A415"/>
+      <c r="F415" s="49"/>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A416"/>
+      <c r="F416" s="49"/>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A417"/>
+      <c r="F417" s="49"/>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A418"/>
+      <c r="F418" s="49"/>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A419"/>
+      <c r="F419" s="49"/>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A420"/>
+      <c r="F420" s="49"/>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A421"/>
+      <c r="F421" s="49"/>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A422"/>
+      <c r="F422" s="49"/>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A423"/>
+      <c r="F423" s="49"/>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424"/>
+      <c r="F424" s="49"/>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A425"/>
+      <c r="F425" s="49"/>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A426"/>
+      <c r="F426" s="49"/>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A427"/>
+      <c r="F427" s="49"/>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A428"/>
+      <c r="F428" s="49"/>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A429"/>
+      <c r="F429" s="49"/>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A430"/>
+      <c r="F430" s="49"/>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A431"/>
+      <c r="F431" s="49"/>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A432"/>
+      <c r="F432" s="49"/>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433"/>
+      <c r="F433" s="49"/>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434"/>
+      <c r="F434" s="49"/>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435"/>
+      <c r="F435" s="49"/>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436"/>
+      <c r="F436" s="49"/>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437"/>
+      <c r="F437" s="49"/>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A438"/>
+      <c r="F438" s="49"/>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439"/>
+      <c r="F439" s="49"/>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440"/>
+      <c r="F440" s="49"/>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441"/>
+      <c r="F441" s="49"/>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442"/>
+      <c r="F442" s="49"/>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A443"/>
+      <c r="F443" s="49"/>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444"/>
+      <c r="F444" s="49"/>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445"/>
+      <c r="F445" s="49"/>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446"/>
+      <c r="F446" s="49"/>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447"/>
+      <c r="F447" s="49"/>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448"/>
+      <c r="F448" s="49"/>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A449"/>
+      <c r="F449" s="49"/>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A450"/>
+      <c r="F450" s="49"/>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A451"/>
+      <c r="F451" s="49"/>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A452"/>
+      <c r="F452" s="49"/>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A453"/>
+      <c r="F453" s="49"/>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A454"/>
+      <c r="F454" s="49"/>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A455"/>
+      <c r="F455" s="49"/>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A456"/>
+      <c r="F456" s="49"/>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A457"/>
+      <c r="F457" s="49"/>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A458"/>
+      <c r="F458" s="49"/>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A459"/>
+      <c r="F459" s="49"/>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A460"/>
+      <c r="F460" s="49"/>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A461"/>
+      <c r="F461" s="49"/>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A462"/>
+      <c r="F462" s="49"/>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A463"/>
+      <c r="F463" s="49"/>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A464"/>
+      <c r="F464" s="49"/>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A465"/>
+      <c r="F465" s="49"/>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A466"/>
+      <c r="F466" s="49"/>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A467"/>
+      <c r="F467" s="49"/>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A468"/>
+      <c r="F468" s="49"/>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469"/>
+      <c r="F469" s="49"/>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470"/>
+      <c r="F470" s="49"/>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A471"/>
+      <c r="F471" s="49"/>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472"/>
+      <c r="F472" s="49"/>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473"/>
+      <c r="F473" s="49"/>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474"/>
+      <c r="F474" s="49"/>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475"/>
+      <c r="F475" s="49"/>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476"/>
+      <c r="F476" s="49"/>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A477"/>
+      <c r="F477" s="49"/>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478"/>
+      <c r="F478" s="49"/>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479"/>
+      <c r="F479" s="49"/>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480"/>
+      <c r="F480" s="49"/>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481"/>
+      <c r="F481" s="49"/>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482"/>
+      <c r="F482" s="49"/>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483"/>
+      <c r="F483" s="49"/>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484"/>
+      <c r="F484" s="49"/>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485"/>
+      <c r="F485" s="49"/>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486"/>
+      <c r="F486" s="49"/>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487"/>
+      <c r="F487" s="49"/>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488"/>
+      <c r="F488" s="49"/>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489"/>
+      <c r="F489" s="49"/>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490"/>
+      <c r="F490" s="49"/>
+    </row>
+    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A491"/>
+      <c r="F491" s="49"/>
+    </row>
+    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A492"/>
+      <c r="F492" s="49"/>
+    </row>
+    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A493"/>
+      <c r="F493" s="49"/>
+    </row>
+    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A494"/>
+      <c r="F494" s="49"/>
+    </row>
+    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A495"/>
+      <c r="F495" s="49"/>
+    </row>
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A496"/>
+      <c r="F496" s="49"/>
+    </row>
+    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A497"/>
+      <c r="F497" s="49"/>
+    </row>
+    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A498"/>
+      <c r="F498" s="49"/>
+    </row>
+    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A499"/>
+      <c r="F499" s="49"/>
+    </row>
+    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A500"/>
+      <c r="F500" s="49"/>
+    </row>
+    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A501"/>
+      <c r="F501" s="49"/>
+    </row>
+    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A502"/>
+      <c r="F502" s="49"/>
+    </row>
+    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A503"/>
+      <c r="F503" s="49"/>
+    </row>
+    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A504"/>
+      <c r="F504" s="49"/>
+    </row>
+    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A505"/>
+      <c r="F505" s="49"/>
+    </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506"/>
+      <c r="F506" s="49"/>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507"/>
+      <c r="F507" s="49"/>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508"/>
+      <c r="F508" s="49"/>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509"/>
+      <c r="F509" s="49"/>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510"/>
+      <c r="F510" s="49"/>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511"/>
+      <c r="F511" s="49"/>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512"/>
+      <c r="F512" s="49"/>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513"/>
+      <c r="F513" s="49"/>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514"/>
+      <c r="F514" s="49"/>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515"/>
+      <c r="F515" s="49"/>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516"/>
+      <c r="F516" s="49"/>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517"/>
+      <c r="F517" s="49"/>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A518"/>
+      <c r="F518" s="49"/>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A519"/>
+      <c r="F519" s="49"/>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520"/>
+      <c r="F520" s="49"/>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521"/>
+      <c r="F521" s="49"/>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522"/>
+      <c r="F522" s="49"/>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A523"/>
+      <c r="F523" s="49"/>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A524"/>
+      <c r="F524" s="49"/>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A525"/>
+      <c r="F525" s="49"/>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A526"/>
+      <c r="F526" s="49"/>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A527"/>
+      <c r="F527" s="49"/>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A528"/>
+      <c r="F528" s="49"/>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A529"/>
+      <c r="F529" s="49"/>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A530"/>
+      <c r="F530" s="49"/>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A531"/>
+      <c r="F531" s="49"/>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A532"/>
+      <c r="F532" s="49"/>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533"/>
+      <c r="F533" s="49"/>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534"/>
+      <c r="F534" s="49"/>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535"/>
+      <c r="F535" s="49"/>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536"/>
+      <c r="F536" s="49"/>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A537"/>
+      <c r="F537" s="49"/>
+    </row>
+    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A538"/>
+      <c r="F538" s="49"/>
+    </row>
+    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A539"/>
+      <c r="F539" s="49"/>
+    </row>
+    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A540"/>
+      <c r="F540" s="49"/>
+    </row>
+    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A541"/>
+      <c r="F541" s="49"/>
+    </row>
+    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A542"/>
+      <c r="F542" s="49"/>
+    </row>
+    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A543"/>
+      <c r="F543" s="49"/>
+    </row>
+    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A544"/>
+      <c r="F544" s="49"/>
+    </row>
+    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A545"/>
+      <c r="F545" s="49"/>
+    </row>
+    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A546"/>
+      <c r="F546" s="49"/>
+    </row>
+    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A547"/>
+      <c r="F547" s="49"/>
+    </row>
+    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A548"/>
+      <c r="F548" s="49"/>
+    </row>
+    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A549"/>
+      <c r="F549" s="49"/>
+    </row>
+    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A550"/>
+      <c r="F550" s="49"/>
+    </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A551"/>
+      <c r="F551" s="49"/>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A552"/>
+      <c r="F552" s="49"/>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A553"/>
+      <c r="F553" s="49"/>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554"/>
+      <c r="F554" s="49"/>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555"/>
+      <c r="F555" s="49"/>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556"/>
+      <c r="F556" s="49"/>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557"/>
+      <c r="F557" s="49"/>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A558"/>
+      <c r="F558" s="49"/>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A559"/>
+      <c r="F559" s="49"/>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A560"/>
+      <c r="F560" s="49"/>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A561"/>
+      <c r="F561" s="49"/>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A562"/>
+      <c r="F562" s="49"/>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A563"/>
+      <c r="F563" s="49"/>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A564"/>
+      <c r="F564" s="49"/>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A565"/>
+      <c r="F565" s="49"/>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A566"/>
+      <c r="F566" s="49"/>
+    </row>
+    <row r="567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A567"/>
+      <c r="F567" s="49"/>
+    </row>
+    <row r="568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A568"/>
+      <c r="F568" s="49"/>
+    </row>
+    <row r="569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A569"/>
+      <c r="F569" s="49"/>
+    </row>
+    <row r="570" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A570"/>
+      <c r="F570" s="49"/>
+    </row>
+    <row r="571" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A571"/>
+      <c r="F571" s="49"/>
+    </row>
+    <row r="572" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A572"/>
+      <c r="F572" s="49"/>
+    </row>
+    <row r="573" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A573"/>
+      <c r="F573" s="49"/>
+    </row>
+    <row r="574" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A574"/>
+      <c r="F574" s="49"/>
+    </row>
+    <row r="575" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A575"/>
+      <c r="F575" s="49"/>
+    </row>
+    <row r="576" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A576"/>
+      <c r="F576" s="49"/>
+    </row>
+    <row r="577" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A577"/>
+      <c r="F577" s="49"/>
+    </row>
+    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A578"/>
+      <c r="F578" s="49"/>
+    </row>
+    <row r="579" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A579"/>
+      <c r="F579" s="49"/>
+    </row>
+    <row r="580" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A580"/>
+      <c r="F580" s="49"/>
+    </row>
+    <row r="581" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A581"/>
+      <c r="F581" s="49"/>
+    </row>
+    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A582"/>
+      <c r="F582" s="49"/>
+    </row>
+    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A583"/>
+      <c r="F583" s="49"/>
+    </row>
+    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A584"/>
+      <c r="F584" s="49"/>
+    </row>
+    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A585"/>
+      <c r="F585" s="49"/>
+    </row>
+    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A586"/>
+      <c r="F586" s="49"/>
+    </row>
+    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A587"/>
+      <c r="F587" s="49"/>
+    </row>
+    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A588"/>
+      <c r="F588" s="49"/>
+    </row>
+    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A589"/>
+      <c r="F589" s="49"/>
+    </row>
+    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A590"/>
+      <c r="F590" s="49"/>
+    </row>
+    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A591"/>
+      <c r="F591" s="49"/>
+    </row>
+    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A592"/>
+      <c r="F592" s="49"/>
+    </row>
+    <row r="593" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A593"/>
+      <c r="F593" s="49"/>
+    </row>
+    <row r="594" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A594"/>
+      <c r="F594" s="49"/>
+    </row>
+    <row r="595" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A595"/>
+      <c r="F595" s="49"/>
+    </row>
+    <row r="596" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A596"/>
+      <c r="F596" s="49"/>
+    </row>
+    <row r="597" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A597"/>
+      <c r="F597" s="49"/>
+    </row>
+    <row r="598" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A598"/>
+      <c r="F598" s="49"/>
+    </row>
+    <row r="599" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A599"/>
+      <c r="F599" s="49"/>
+    </row>
+    <row r="600" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A600"/>
+      <c r="F600" s="49"/>
+    </row>
+    <row r="601" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A601"/>
+      <c r="F601" s="49"/>
+    </row>
+    <row r="602" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A602"/>
+      <c r="F602" s="49"/>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A603"/>
+      <c r="F603" s="49"/>
+    </row>
+    <row r="604" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A604"/>
+      <c r="F604" s="49"/>
+    </row>
+    <row r="605" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A605"/>
+      <c r="F605" s="49"/>
+    </row>
+    <row r="606" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A606"/>
+      <c r="F606" s="49"/>
+    </row>
+    <row r="607" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A607"/>
+      <c r="F607" s="49"/>
+    </row>
+    <row r="608" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A608"/>
+      <c r="F608" s="49"/>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A609"/>
+      <c r="F609" s="49"/>
+    </row>
+    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A610"/>
+      <c r="F610" s="49"/>
+    </row>
+    <row r="611" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A611"/>
+      <c r="F611" s="49"/>
+    </row>
+    <row r="612" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A612"/>
+      <c r="F612" s="49"/>
+    </row>
+    <row r="613" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A613"/>
+      <c r="F613" s="49"/>
+    </row>
+    <row r="614" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A614"/>
+      <c r="F614" s="49"/>
+    </row>
+    <row r="615" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A615"/>
+      <c r="F615" s="49"/>
+    </row>
+    <row r="616" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A616"/>
+      <c r="F616" s="49"/>
+    </row>
+    <row r="617" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A617"/>
+      <c r="F617" s="49"/>
+    </row>
+    <row r="618" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A618"/>
+      <c r="F618" s="49"/>
+    </row>
+    <row r="619" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A619"/>
+      <c r="F619" s="49"/>
+    </row>
+    <row r="620" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A620"/>
+      <c r="F620" s="49"/>
+    </row>
+    <row r="621" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A621"/>
+      <c r="F621" s="49"/>
+    </row>
+    <row r="622" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A622"/>
+      <c r="F622" s="49"/>
+    </row>
+    <row r="623" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A623"/>
+      <c r="F623" s="49"/>
+    </row>
+    <row r="624" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A624"/>
+      <c r="F624" s="49"/>
+    </row>
+    <row r="625" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A625"/>
+      <c r="F625" s="49"/>
+    </row>
+    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A626"/>
+      <c r="F626" s="49"/>
+    </row>
+    <row r="627" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A627"/>
+      <c r="F627" s="49"/>
+    </row>
+    <row r="628" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A628"/>
+      <c r="F628" s="49"/>
+    </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A629"/>
+      <c r="F629" s="49"/>
+    </row>
+    <row r="630" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A630"/>
+      <c r="F630" s="49"/>
+    </row>
+    <row r="631" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A631"/>
+      <c r="F631" s="49"/>
+    </row>
+    <row r="632" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A632"/>
+      <c r="F632" s="49"/>
+    </row>
+    <row r="633" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A633"/>
+      <c r="F633" s="49"/>
+    </row>
+    <row r="634" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A634"/>
+      <c r="F634" s="49"/>
+    </row>
+    <row r="635" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A635"/>
+      <c r="F635" s="49"/>
+    </row>
+    <row r="636" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A636"/>
+      <c r="F636" s="49"/>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A637"/>
+      <c r="F637" s="49"/>
+    </row>
+    <row r="638" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A638"/>
+      <c r="F638" s="49"/>
+    </row>
+    <row r="639" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A639"/>
+      <c r="F639" s="49"/>
+    </row>
+    <row r="640" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A640"/>
+      <c r="F640" s="49"/>
+    </row>
+    <row r="641" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A641"/>
+      <c r="F641" s="49"/>
+    </row>
+    <row r="642" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A642"/>
+      <c r="F642" s="49"/>
+    </row>
+    <row r="643" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A643"/>
+      <c r="F643" s="49"/>
+    </row>
+    <row r="644" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A644"/>
+      <c r="F644" s="49"/>
+    </row>
+    <row r="645" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A645"/>
+      <c r="F645" s="49"/>
+    </row>
+    <row r="646" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A646"/>
+      <c r="F646" s="49"/>
+    </row>
+    <row r="647" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A647"/>
+      <c r="F647" s="49"/>
+    </row>
+    <row r="648" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A648"/>
+      <c r="F648" s="49"/>
+    </row>
+    <row r="649" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A649"/>
+      <c r="F649" s="49"/>
+    </row>
+    <row r="650" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A650"/>
+      <c r="F650" s="49"/>
+    </row>
+    <row r="651" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A651"/>
+      <c r="F651" s="49"/>
+    </row>
+    <row r="652" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A652"/>
+      <c r="F652" s="49"/>
+    </row>
+    <row r="653" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A653"/>
+      <c r="F653" s="49"/>
+    </row>
+    <row r="654" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A654"/>
+      <c r="F654" s="49"/>
+    </row>
+    <row r="655" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A655"/>
+      <c r="F655" s="49"/>
+    </row>
+    <row r="656" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A656"/>
+      <c r="F656" s="49"/>
+    </row>
+    <row r="657" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A657"/>
+      <c r="F657" s="49"/>
+    </row>
+    <row r="658" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A658"/>
+      <c r="F658" s="49"/>
+    </row>
+    <row r="659" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A659"/>
+      <c r="F659" s="49"/>
+    </row>
+    <row r="660" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A660"/>
+      <c r="F660" s="49"/>
+    </row>
+    <row r="661" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A661"/>
+      <c r="F661" s="49"/>
+    </row>
+    <row r="662" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A662"/>
+      <c r="F662" s="49"/>
+    </row>
+    <row r="663" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A663"/>
+      <c r="F663" s="49"/>
+    </row>
+    <row r="664" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A664"/>
+      <c r="F664" s="49"/>
+    </row>
+    <row r="665" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A665"/>
+      <c r="F665" s="49"/>
+    </row>
+    <row r="666" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A666"/>
+      <c r="F666" s="49"/>
+    </row>
+    <row r="667" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A667"/>
+      <c r="F667" s="49"/>
+    </row>
+    <row r="668" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A668"/>
+      <c r="F668" s="49"/>
+    </row>
+    <row r="669" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A669"/>
+      <c r="F669" s="49"/>
+    </row>
+    <row r="670" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A670"/>
+      <c r="F670" s="49"/>
+    </row>
+    <row r="671" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A671"/>
+      <c r="F671" s="49"/>
+    </row>
+    <row r="672" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A672"/>
+      <c r="F672" s="49"/>
+    </row>
+    <row r="673" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A673"/>
+      <c r="F673" s="49"/>
+    </row>
+    <row r="674" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A674"/>
+      <c r="F674" s="49"/>
+    </row>
+    <row r="675" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A675"/>
+      <c r="F675" s="49"/>
+    </row>
+    <row r="676" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A676"/>
+      <c r="F676" s="49"/>
+    </row>
+    <row r="677" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A677"/>
+      <c r="F677" s="49"/>
+    </row>
+    <row r="678" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A678"/>
+      <c r="F678" s="49"/>
+    </row>
+    <row r="679" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A679"/>
+      <c r="F679" s="49"/>
+    </row>
+    <row r="680" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A680"/>
+      <c r="F680" s="49"/>
+    </row>
+    <row r="681" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A681"/>
+      <c r="F681" s="49"/>
+    </row>
+    <row r="682" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A682"/>
+      <c r="F682" s="49"/>
+    </row>
+    <row r="683" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A683"/>
+      <c r="F683" s="49"/>
+    </row>
+    <row r="684" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A684"/>
+      <c r="F684" s="49"/>
+    </row>
+    <row r="685" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A685"/>
+      <c r="F685" s="49"/>
+    </row>
+    <row r="686" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A686"/>
+      <c r="F686" s="49"/>
+    </row>
+    <row r="687" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A687"/>
+      <c r="F687" s="49"/>
+    </row>
+    <row r="688" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A688"/>
+      <c r="F688" s="49"/>
+    </row>
+    <row r="689" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A689"/>
+      <c r="F689" s="49"/>
+    </row>
+    <row r="690" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A690"/>
+      <c r="F690" s="49"/>
+    </row>
+    <row r="691" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A691"/>
+      <c r="F691" s="49"/>
+    </row>
+    <row r="692" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A692"/>
+      <c r="F692" s="49"/>
+    </row>
+    <row r="693" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A693"/>
+      <c r="F693" s="49"/>
+    </row>
+    <row r="694" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A694"/>
+      <c r="F694" s="49"/>
+    </row>
+    <row r="695" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A695"/>
+      <c r="F695" s="49"/>
+    </row>
+    <row r="696" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A696"/>
+      <c r="F696" s="49"/>
+    </row>
+    <row r="697" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A697"/>
+      <c r="F697" s="49"/>
+    </row>
+    <row r="698" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A698"/>
+      <c r="F698" s="49"/>
+    </row>
+    <row r="699" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A699"/>
+      <c r="F699" s="49"/>
+    </row>
+    <row r="700" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A700"/>
+      <c r="F700" s="49"/>
+    </row>
+    <row r="701" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A701"/>
+      <c r="F701" s="49"/>
+    </row>
+    <row r="702" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A702"/>
+      <c r="F702" s="49"/>
+    </row>
+    <row r="703" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A703"/>
+      <c r="F703" s="49"/>
+    </row>
+    <row r="704" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A704"/>
+      <c r="F704" s="49"/>
+    </row>
+    <row r="705" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A705"/>
+      <c r="F705" s="49"/>
+    </row>
+    <row r="706" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A706"/>
+      <c r="F706" s="49"/>
+    </row>
+    <row r="707" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A707"/>
+      <c r="F707" s="49"/>
+    </row>
+    <row r="708" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A708"/>
+      <c r="F708" s="49"/>
+    </row>
+    <row r="709" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A709"/>
+      <c r="F709" s="49"/>
+    </row>
+    <row r="710" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A710"/>
+      <c r="F710" s="49"/>
+    </row>
+    <row r="711" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A711"/>
+      <c r="F711" s="49"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{1907E72F-7CBD-4F98-B8E1-12C429478408}">
+      <formula1>"?, kcal*Å^6/mol, kJ*nm^6/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{66A2AA09-FFF2-4253-A232-47730CDCE5DD}">
+      <formula1>$B$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{CAD532F9-F5E9-4E27-BC59-1FD2F7042D59}">
+      <formula1>"Lennard-Jones (12-6) [A-B Form]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{B5E8CEAD-FE17-494A-A364-77D1D37E2F18}">
+      <formula1>"?, kcal*Å^12/mol, kJ*nm^12/mol"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2700,7 +5657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2819,7 +5776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2840,12 +5797,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3034,125 +5991,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1200-000000000000}">
-      <formula1>"?, Å, nm"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1200-000001000000}">
-      <formula1>"?, kcal/mol, kJ/mol"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1200-000002000000}">
-      <formula1>"4*epsilon*[((sigma/R)^-12)-((sigma/R)^-6)+(1/4)]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1200-000003000000}">
-      <formula1>"Weeks-Chandler-Anderson"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3176,10 +6014,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="45"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -3295,6 +6133,125 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1200-000000000000}">
+      <formula1>"?, Å, nm"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1200-000001000000}">
+      <formula1>"?, kcal/mol, kJ/mol"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1200-000002000000}">
+      <formula1>"4*epsilon*[((sigma/R)^-12)-((sigma/R)^-6)+(1/4)]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1200-000003000000}">
+      <formula1>"Weeks-Chandler-Anderson"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -3421,7 +6378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -3576,7 +6533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -3680,7 +6637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -3813,7 +6770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -3928,7 +6885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -3952,16 +6909,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4076,7 +7033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -4099,13 +7056,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4638,15 +7595,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -4794,12 +7751,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -4993,15 +7950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -5152,17 +8109,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -5286,17 +8243,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -5423,16 +8380,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
Added References Metadata section
</commit_message>
<xml_diff>
--- a/XML/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
+++ b/XML/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
@@ -8,39 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Projects\WebFF-Documentation\XML\Coarse-Grained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68E0964F-BB0B-4B9D-8A6E-D9BA0752FFA1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCB51E7C-42DA-4096-BD4A-BA94E96CE772}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
     <sheet name="Keywords" sheetId="21" r:id="rId2"/>
     <sheet name="KeywordsList" sheetId="36" state="hidden" r:id="rId3"/>
-    <sheet name="BondPotential-Harmonic" sheetId="38" r:id="rId4"/>
-    <sheet name="BondPotential-Tabular" sheetId="1" r:id="rId5"/>
-    <sheet name="BondPotential-FENE" sheetId="39" r:id="rId6"/>
-    <sheet name="AnglePotential-Harmonic" sheetId="40" r:id="rId7"/>
-    <sheet name="AnglePotential-COS2" sheetId="41" r:id="rId8"/>
-    <sheet name="AnglePotential-Cosine" sheetId="54" r:id="rId9"/>
-    <sheet name="AnglePotential-Tabular" sheetId="8" r:id="rId10"/>
-    <sheet name="DihedralPotential-CHARMM" sheetId="57" r:id="rId11"/>
-    <sheet name="DihedralPotential-Quadratic" sheetId="42" r:id="rId12"/>
-    <sheet name="DihedralPotential-Tabular" sheetId="11" r:id="rId13"/>
-    <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId14"/>
-    <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId15"/>
-    <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId16"/>
-    <sheet name="NonBondPotential-LJ-AB" sheetId="56" r:id="rId17"/>
-    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId18"/>
-    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId19"/>
-    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId20"/>
-    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId21"/>
-    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId22"/>
-    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId23"/>
-    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId24"/>
-    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId25"/>
-    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId26"/>
-    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId27"/>
-    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId28"/>
+    <sheet name="References" sheetId="58" r:id="rId4"/>
+    <sheet name="BondPotential-Harmonic" sheetId="38" r:id="rId5"/>
+    <sheet name="BondPotential-Tabular" sheetId="1" r:id="rId6"/>
+    <sheet name="BondPotential-FENE" sheetId="39" r:id="rId7"/>
+    <sheet name="AnglePotential-Harmonic" sheetId="40" r:id="rId8"/>
+    <sheet name="AnglePotential-COS2" sheetId="41" r:id="rId9"/>
+    <sheet name="AnglePotential-Cosine" sheetId="54" r:id="rId10"/>
+    <sheet name="AnglePotential-Tabular" sheetId="8" r:id="rId11"/>
+    <sheet name="DihedralPotential-CHARMM" sheetId="57" r:id="rId12"/>
+    <sheet name="DihedralPotential-Quadratic" sheetId="42" r:id="rId13"/>
+    <sheet name="DihedralPotential-Tabular" sheetId="11" r:id="rId14"/>
+    <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId15"/>
+    <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId16"/>
+    <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId17"/>
+    <sheet name="NonBondPotential-LJ-AB" sheetId="56" r:id="rId18"/>
+    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId19"/>
+    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId20"/>
+    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId21"/>
+    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId22"/>
+    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId23"/>
+    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId24"/>
+    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId25"/>
+    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId26"/>
+    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId27"/>
+    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId28"/>
+    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId29"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="256">
   <si>
     <t>AT-1</t>
   </si>
@@ -816,6 +817,21 @@
   </si>
   <si>
     <t>#Choose</t>
+  </si>
+  <si>
+    <t>Additional References</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>DOI</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -950,7 +966,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1066,6 +1082,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1077,7 +1130,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1159,6 +1212,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1168,7 +1222,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1523,22 +1603,22 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.59765625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="52" style="21" customWidth="1"/>
+    <col min="2" max="2" width="75.73046875" style="21" customWidth="1"/>
     <col min="3" max="16384" width="9.1328125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="47"/>
+      <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
@@ -1584,13 +1664,13 @@
       </c>
       <c r="B9" s="25"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="50" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="26"/>
     </row>
-    <row r="11" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="23" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1680,7 @@
       <c r="A12" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="31"/>
     </row>
     <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="23" t="s">
@@ -1644,6 +1724,124 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.265625" customWidth="1"/>
+    <col min="2" max="2" width="18.86328125" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" customWidth="1"/>
+    <col min="6" max="6" width="34.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.73046875" customWidth="1"/>
+    <col min="8" max="8" width="15.1328125" customWidth="1"/>
+    <col min="9" max="16384" width="9.1328125" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="7" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0800-000000000000}">
+      <formula1>"Cosine"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0800-000001000000}">
+      <formula1>"Ka*[1+cos(theta)]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0800-000002000000}">
+      <formula1>"?,kcal,Joules,Reduced"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -1665,12 +1863,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -1849,14 +2047,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E562CDE4-C63C-4524-B913-A40AA59D862E}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -1972,19 +2170,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="F10" s="50"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="F11" s="50"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="F12" s="50"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="F13" s="50"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="F14" s="50"/>
+      <c r="F14" s="47"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2009,7 +2207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -2148,7 +2346,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -2168,12 +2366,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -2375,7 +2573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
@@ -2513,7 +2711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2638,7 +2836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -2659,15 +2857,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -2773,7 +2971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E701295-13E7-4A34-A798-03BF4464E0DA}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -5698,7 +5896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -5828,125 +6026,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="36.1328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="8" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1000-000000000000}">
-      <formula1>"Lennard-Jones (9-6) [Class 2 Form]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1000-000001000000}">
-      <formula1>"epsilon*[2*(sigma/R)^9-3*(sigma/R)^6]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1000-000002000000}">
-      <formula1>"?,kcal/mol,kJ/mol,Reduced"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1000-000003000000}">
-      <formula1>"?,Å,nm,Reduced"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -5956,7 +6035,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5967,10 +6046,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="49"/>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
@@ -6086,6 +6165,125 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="8" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1000-000000000000}">
+      <formula1>"Lennard-Jones (9-6) [Class 2 Form]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-1000-000001000000}">
+      <formula1>"epsilon*[2*(sigma/R)^9-3*(sigma/R)^6]"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-1000-000002000000}">
+      <formula1>"?,kcal/mol,kJ/mol,Reduced"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{00000000-0002-0000-1000-000003000000}">
+      <formula1>"?,Å,nm,Reduced"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -6106,12 +6304,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -6303,7 +6501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -6422,7 +6620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -6549,7 +6747,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -6704,7 +6902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -6808,7 +7006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -6941,7 +7139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -7056,7 +7254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -7080,16 +7278,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -7204,7 +7402,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -7227,13 +7425,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -7743,6 +7941,187 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E1CE25-A0B8-4CC6-A1A0-17C4F6DD7775}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="75.1328125" customWidth="1"/>
+    <col min="2" max="2" width="25.1328125" customWidth="1"/>
+    <col min="3" max="3" width="39.73046875" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="53"/>
+    </row>
+    <row r="3" spans="1:4" ht="25.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="55" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="56"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="54"/>
+    </row>
+    <row r="5" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="58"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="25"/>
+    </row>
+    <row r="12" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="25"/>
+    </row>
+    <row r="13" spans="1:4" ht="50" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+    </row>
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7766,15 +8145,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
@@ -7899,7 +8278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7922,12 +8301,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -8097,7 +8476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -8121,15 +8500,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
@@ -8254,7 +8633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -8280,17 +8659,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -8388,7 +8767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -8414,17 +8793,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
@@ -8524,122 +8903,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <tabColor theme="5"/>
-  </sheetPr>
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="16.265625" customWidth="1"/>
-    <col min="2" max="2" width="18.86328125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" customWidth="1"/>
-    <col min="6" max="6" width="34.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" customWidth="1"/>
-    <col min="8" max="8" width="15.1328125" customWidth="1"/>
-    <col min="9" max="16384" width="9.1328125" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="30.75" x14ac:dyDescent="0.9">
-      <c r="A1" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="7" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0800-000000000000}">
-      <formula1>"Cosine"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{00000000-0002-0000-0800-000001000000}">
-      <formula1>"Ka*[1+cos(theta)]"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{00000000-0002-0000-0800-000002000000}">
-      <formula1>"?,kcal,Joules,Reduced"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed font and added hover comments for Dihedral Multiharmonic
</commit_message>
<xml_diff>
--- a/XML/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
+++ b/XML/Coarse-Grained/WebFF-CoarseGrained-DataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Projects\WebFF-Documentation\XML\Coarse-Grained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BC0DBF-F9D4-47B9-9ED3-7C0592CBAE10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6010F52A-4B81-4FE7-8E16-EBE226A731F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14010" windowHeight="8190" tabRatio="908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="908" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="20" r:id="rId1"/>
@@ -26,22 +26,23 @@
     <sheet name="AnglePotential-Tabular" sheetId="8" r:id="rId11"/>
     <sheet name="DihedralPotential-CHARMM" sheetId="57" r:id="rId12"/>
     <sheet name="DihedralPotential-Quadratic" sheetId="42" r:id="rId13"/>
-    <sheet name="DihedralPotential-Tabular" sheetId="11" r:id="rId14"/>
-    <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId15"/>
-    <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId16"/>
-    <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId17"/>
-    <sheet name="NonBondPotential-LJ2-AB" sheetId="56" r:id="rId18"/>
-    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId19"/>
-    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId20"/>
-    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId21"/>
-    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId22"/>
-    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId23"/>
-    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId24"/>
-    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId25"/>
-    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId26"/>
-    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId27"/>
-    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId28"/>
-    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId29"/>
+    <sheet name="DihedralPotential-Multiharmonic" sheetId="60" r:id="rId14"/>
+    <sheet name="DihedralPotential-Tabular" sheetId="11" r:id="rId15"/>
+    <sheet name="ImproperPotential-Harmonic" sheetId="43" r:id="rId16"/>
+    <sheet name="NonBondPotential-LJ" sheetId="44" r:id="rId17"/>
+    <sheet name="NonBondPotential-LJ2" sheetId="45" r:id="rId18"/>
+    <sheet name="NonBondPotential-LJ2-AB" sheetId="56" r:id="rId19"/>
+    <sheet name="NonBondPotential-LJ96" sheetId="46" r:id="rId20"/>
+    <sheet name="NonBondPotential-LJ962" sheetId="55" r:id="rId21"/>
+    <sheet name="NonBondPotential-Tabular" sheetId="22" r:id="rId22"/>
+    <sheet name="NonBondPotential-WCA" sheetId="47" r:id="rId23"/>
+    <sheet name="NonBondPotential-Mie" sheetId="48" r:id="rId24"/>
+    <sheet name="NonBondPotential-EnergyRenorm" sheetId="49" r:id="rId25"/>
+    <sheet name="DissipativePotential-Langevin" sheetId="50" r:id="rId26"/>
+    <sheet name="SoftPotential-DPD" sheetId="52" r:id="rId27"/>
+    <sheet name="SoftPotential-SRP" sheetId="53" r:id="rId28"/>
+    <sheet name="AtomType-ATDL" sheetId="30" r:id="rId29"/>
+    <sheet name="AtomType-CoarseGrained" sheetId="51" r:id="rId30"/>
   </sheets>
   <definedNames>
     <definedName name="KeywordListTab_1" localSheetId="2">KeywordsList!$A$2:$A$74</definedName>
@@ -793,7 +794,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{F881B717-D92F-4832-BB50-91F490BFAF2D}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7BCFF6A5-A792-43B3-A547-B6FD15D16AC9}">
       <text>
         <r>
           <rPr>
@@ -805,19 +806,9 @@
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{9BFA1C26-BF1B-4223-9FD0-198FA2B93CBA}">
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{1016CD91-14DF-46CE-8E88-282690D42027}">
       <text>
         <r>
           <rPr>
@@ -829,19 +820,9 @@
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{23A77A13-F7D7-47E5-8E4A-C628FC0EDB8A}">
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{F8FA30B3-ECF5-49A0-AAE9-44946419B0E5}">
       <text>
         <r>
           <rPr>
@@ -853,19 +834,9 @@
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B98B07F2-96F3-4D91-AEE3-2CFC16F409FE}">
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{CC4BE0F2-9739-4DD8-AA4D-D8D91B14DF4E}">
       <text>
         <r>
           <rPr>
@@ -877,91 +848,9 @@
           </rPr>
           <t>Attribute data, required entry</t>
         </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{79D907D3-1919-4607-89C8-2AE9387227D7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional attribute data, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{FEF2A91F-066E-48AD-B971-4F1454D112CB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional attribute data, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{4DDA661E-B200-4C0B-9684-9E4BDEB9D3ED}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional attribute data, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{643CFA18-C2F3-411E-AA0F-1D1A134F8815}">
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{6C37F546-5222-4159-953A-98016F80BD4E}">
       <text>
         <r>
           <rPr>
@@ -985,7 +874,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{7EBB6ABB-5F80-48D1-9059-B649A11BDE28}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{597362C2-A747-4AEC-B79F-1E2EA6713083}">
       <text>
         <r>
           <rPr>
@@ -1009,7 +898,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{6AEFFFE6-E507-483B-980D-EEB536189240}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{52305B25-10C0-47CC-94C7-604D19754381}">
       <text>
         <r>
           <rPr>
@@ -1029,6 +918,96 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00D45898-4869-4F1F-B478-C37A28C8E9A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{8D8A4C33-779D-4958-B6BA-9F5F2D191DC1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{C0F9A26A-3876-4575-BC92-EE0A58D540F2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional attribute data, not required
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{F86CF249-F079-457D-8D55-BD21B9A9536D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional attribute data, not required
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{8CA36530-25F1-4FC5-A057-638694006BE5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Optional attribute data, not required
 </t>
         </r>
       </text>
@@ -1043,7 +1022,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{A02E6D57-3DC5-4213-9839-61F3FCEAB5B2}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{F881B717-D92F-4832-BB50-91F490BFAF2D}">
       <text>
         <r>
           <rPr>
@@ -1067,7 +1046,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{C43539B6-3162-4372-8B49-662350522BCF}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{9BFA1C26-BF1B-4223-9FD0-198FA2B93CBA}">
       <text>
         <r>
           <rPr>
@@ -1091,7 +1070,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{91F2C4DB-1E40-4FDE-A697-0C44ADAF1E2D}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{23A77A13-F7D7-47E5-8E4A-C628FC0EDB8A}">
       <text>
         <r>
           <rPr>
@@ -1115,7 +1094,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{65BBE8CD-0B51-46DF-B6DB-23A72A1965FF}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{B98B07F2-96F3-4D91-AEE3-2CFC16F409FE}">
       <text>
         <r>
           <rPr>
@@ -1139,31 +1118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{FE5F04F9-E6BE-4732-A322-E813BA2856CD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attribute data, required entry</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{80E295C1-701A-4EFC-A29E-C6453A9CA21F}">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{79D907D3-1919-4607-89C8-2AE9387227D7}">
       <text>
         <r>
           <rPr>
@@ -1187,7 +1142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{4AF130E1-6D88-43B2-9D4E-67238B33387B}">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{FEF2A91F-066E-48AD-B971-4F1454D112CB}">
       <text>
         <r>
           <rPr>
@@ -1211,7 +1166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{B9F62766-D949-45C2-B90A-0345C01AEB48}">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{4DDA661E-B200-4C0B-9684-9E4BDEB9D3ED}">
       <text>
         <r>
           <rPr>
@@ -1222,6 +1177,78 @@
             <family val="2"/>
           </rPr>
           <t>Optional attribute data, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{643CFA18-C2F3-411E-AA0F-1D1A134F8815}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{7EBB6ABB-5F80-48D1-9059-B649A11BDE28}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{6AEFFFE6-E507-483B-980D-EEB536189240}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
         </r>
         <r>
           <rPr>
@@ -1245,7 +1272,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1B8741C1-6B2C-4911-89CC-7F2AF05E173D}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{A02E6D57-3DC5-4213-9839-61F3FCEAB5B2}">
       <text>
         <r>
           <rPr>
@@ -1269,7 +1296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{3DE3A8AD-8040-4508-B793-3AE35E915126}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{C43539B6-3162-4372-8B49-662350522BCF}">
       <text>
         <r>
           <rPr>
@@ -1293,7 +1320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{D7D6E744-40A7-4460-B36E-3AAB30DC1491}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{91F2C4DB-1E40-4FDE-A697-0C44ADAF1E2D}">
       <text>
         <r>
           <rPr>
@@ -1317,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{ABDB4384-15FD-4874-A296-E1DB0663B850}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{65BBE8CD-0B51-46DF-B6DB-23A72A1965FF}">
       <text>
         <r>
           <rPr>
@@ -1341,7 +1368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{D182A99A-6A73-4316-9E02-DB7A1146974E}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{FE5F04F9-E6BE-4732-A322-E813BA2856CD}">
       <text>
         <r>
           <rPr>
@@ -1365,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{D9414062-4FF1-4D1D-9EE8-4EC4B27ECFCF}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{80E295C1-701A-4EFC-A29E-C6453A9CA21F}">
       <text>
         <r>
           <rPr>
@@ -1389,7 +1416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{35C0E02D-82A7-4C48-A68B-FBE52AF10CEE}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{4AF130E1-6D88-43B2-9D4E-67238B33387B}">
       <text>
         <r>
           <rPr>
@@ -1413,7 +1440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{99933E6A-1F75-4CAC-B31A-CC4CC304D301}">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{B9F62766-D949-45C2-B90A-0345C01AEB48}">
       <text>
         <r>
           <rPr>
@@ -1447,7 +1474,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{B350E927-0367-4469-A3E7-338BE9099F2D}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1B8741C1-6B2C-4911-89CC-7F2AF05E173D}">
       <text>
         <r>
           <rPr>
@@ -1471,7 +1498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{05AEE0E8-897A-47BA-A5FE-6E3A6CD16D2A}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{3DE3A8AD-8040-4508-B793-3AE35E915126}">
       <text>
         <r>
           <rPr>
@@ -1495,7 +1522,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{B4FE2DD1-222A-4CA6-9076-F24B0FD2DCE4}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{D7D6E744-40A7-4460-B36E-3AAB30DC1491}">
       <text>
         <r>
           <rPr>
@@ -1519,7 +1546,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{E1EBF96A-D773-4E52-BC9E-BF3F875EB304}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{ABDB4384-15FD-4874-A296-E1DB0663B850}">
       <text>
         <r>
           <rPr>
@@ -1543,7 +1570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{0A659294-D96A-44EA-9319-B894BE7066FA}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{D182A99A-6A73-4316-9E02-DB7A1146974E}">
       <text>
         <r>
           <rPr>
@@ -1567,7 +1594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{01766876-A49C-48D3-AF69-B786BB45D130}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{D9414062-4FF1-4D1D-9EE8-4EC4B27ECFCF}">
       <text>
         <r>
           <rPr>
@@ -1591,7 +1618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{B80862F3-53B8-469B-B3E9-429539AB430F}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{35C0E02D-82A7-4C48-A68B-FBE52AF10CEE}">
       <text>
         <r>
           <rPr>
@@ -1615,7 +1642,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{AE9906B6-F156-4845-9C41-7DFB08F3EEB5}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{99933E6A-1F75-4CAC-B31A-CC4CC304D301}">
       <text>
         <r>
           <rPr>
@@ -1649,7 +1676,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{994EEB6E-6F56-4FD9-8775-E4D9EDE66522}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{B350E927-0367-4469-A3E7-338BE9099F2D}">
       <text>
         <r>
           <rPr>
@@ -1673,7 +1700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{DA50AE37-FE59-469C-BE1B-2188B272191B}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{05AEE0E8-897A-47BA-A5FE-6E3A6CD16D2A}">
       <text>
         <r>
           <rPr>
@@ -1697,7 +1724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{596D2958-F935-4CA6-AC72-887D8FC4CE00}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{B4FE2DD1-222A-4CA6-9076-F24B0FD2DCE4}">
       <text>
         <r>
           <rPr>
@@ -1721,7 +1748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{CF2F795E-07C3-4F3C-9ED3-2934BE14BA81}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{E1EBF96A-D773-4E52-BC9E-BF3F875EB304}">
       <text>
         <r>
           <rPr>
@@ -1745,7 +1772,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{7038E2F8-4B51-4987-8F6F-09519E8A4683}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{0A659294-D96A-44EA-9319-B894BE7066FA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{01766876-A49C-48D3-AF69-B786BB45D130}">
       <text>
         <r>
           <rPr>
@@ -1769,7 +1820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{ABB79B6A-26FE-4D30-9EFE-889AF6A6FFF4}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{B80862F3-53B8-469B-B3E9-429539AB430F}">
       <text>
         <r>
           <rPr>
@@ -1793,7 +1844,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{F5D0EE42-07FC-4241-BA30-8FDA641B97A7}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{AE9906B6-F156-4845-9C41-7DFB08F3EEB5}">
       <text>
         <r>
           <rPr>
@@ -1827,7 +1878,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DBDCA9C1-AF4E-471E-B0E0-07E2E605D85D}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{994EEB6E-6F56-4FD9-8775-E4D9EDE66522}">
       <text>
         <r>
           <rPr>
@@ -1851,7 +1902,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{81478D69-FE51-4A75-93E7-121AFDCE50B4}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{DA50AE37-FE59-469C-BE1B-2188B272191B}">
       <text>
         <r>
           <rPr>
@@ -1875,7 +1926,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{BE25CF8E-B884-4FDB-8961-2B88B2204B6F}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{596D2958-F935-4CA6-AC72-887D8FC4CE00}">
       <text>
         <r>
           <rPr>
@@ -1899,7 +1950,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{45AFE056-901C-4B93-9887-DA554D908801}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{CF2F795E-07C3-4F3C-9ED3-2934BE14BA81}">
       <text>
         <r>
           <rPr>
@@ -1923,31 +1974,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{3F9C3BF3-34EF-4014-9AE8-36F1ABEF4015}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attribute data, required entry</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{655DC909-7573-42F1-AD88-269640FB20A1}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{7038E2F8-4B51-4987-8F6F-09519E8A4683}">
       <text>
         <r>
           <rPr>
@@ -1971,7 +1998,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{CF4CCBDF-4A98-495B-8CD3-2D6364CB697B}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{ABB79B6A-26FE-4D30-9EFE-889AF6A6FFF4}">
       <text>
         <r>
           <rPr>
@@ -1995,7 +2022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{A72BFA40-D5B0-4CBE-A632-ED65E8D26CE9}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{F5D0EE42-07FC-4241-BA30-8FDA641B97A7}">
       <text>
         <r>
           <rPr>
@@ -2029,7 +2056,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{61D77E1D-8C9F-4BDB-B880-53BE9DE2F0C6}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DBDCA9C1-AF4E-471E-B0E0-07E2E605D85D}">
       <text>
         <r>
           <rPr>
@@ -2053,7 +2080,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{637FB3EE-887B-4C00-94FC-8259D1F7084A}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{81478D69-FE51-4A75-93E7-121AFDCE50B4}">
       <text>
         <r>
           <rPr>
@@ -2077,7 +2104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{2B05FDFA-625A-40ED-94D9-5AB2DFA1DA0A}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{BE25CF8E-B884-4FDB-8961-2B88B2204B6F}">
       <text>
         <r>
           <rPr>
@@ -2101,7 +2128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{3247F4A9-213B-4DBC-9363-5CF5858E245C}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{45AFE056-901C-4B93-9887-DA554D908801}">
       <text>
         <r>
           <rPr>
@@ -2125,7 +2152,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{D4DD520C-B4EA-49D9-8876-BB85B4FD6B30}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{3F9C3BF3-34EF-4014-9AE8-36F1ABEF4015}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{655DC909-7573-42F1-AD88-269640FB20A1}">
       <text>
         <r>
           <rPr>
@@ -2149,7 +2200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{4FFA0EB3-73C7-4ED7-8C7C-A5BA82E13392}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{CF4CCBDF-4A98-495B-8CD3-2D6364CB697B}">
       <text>
         <r>
           <rPr>
@@ -2173,7 +2224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{688B99D5-A969-4605-AEBB-7A9642077CA1}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{A72BFA40-D5B0-4CBE-A632-ED65E8D26CE9}">
       <text>
         <r>
           <rPr>
@@ -2241,7 +2292,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{D7411B94-0C0A-415E-91F2-7398B2DD464F}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{61D77E1D-8C9F-4BDB-B880-53BE9DE2F0C6}">
       <text>
         <r>
           <rPr>
@@ -2265,7 +2316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A46E5A54-3492-4CC4-995C-41890EF3A9FB}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{637FB3EE-887B-4C00-94FC-8259D1F7084A}">
       <text>
         <r>
           <rPr>
@@ -2289,7 +2340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{AF8E8A0D-8218-4BE3-8F4E-F775F7661895}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{2B05FDFA-625A-40ED-94D9-5AB2DFA1DA0A}">
       <text>
         <r>
           <rPr>
@@ -2313,7 +2364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{39AB6324-F68A-4B7B-ADA6-8AD3F2BB0D09}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{3247F4A9-213B-4DBC-9363-5CF5858E245C}">
       <text>
         <r>
           <rPr>
@@ -2337,31 +2388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{667BC901-3704-427A-A0DF-0ED43F631931}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attribute data, required entry</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{2313F2F1-29B0-465C-9B3D-C40960FC0CA1}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{D4DD520C-B4EA-49D9-8876-BB85B4FD6B30}">
       <text>
         <r>
           <rPr>
@@ -2385,7 +2412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{3667D5C3-09C7-451C-89F9-331BBCB3A653}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{4FFA0EB3-73C7-4ED7-8C7C-A5BA82E13392}">
       <text>
         <r>
           <rPr>
@@ -2409,7 +2436,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{34875AEB-942F-4EED-8EA9-1B30042F5015}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{688B99D5-A969-4605-AEBB-7A9642077CA1}">
       <text>
         <r>
           <rPr>
@@ -2420,102 +2447,6 @@
             <family val="2"/>
           </rPr>
           <t>Optional attribute data, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{0579E43D-B7E6-4954-8A5F-D03F3260A9FF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional entry, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{57431432-2C56-4F07-8188-C465BAA3E506}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional entry, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{9A550AEE-CC74-407E-845A-CFFF6CAEF797}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional entry, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{C73CE28E-AFC3-4296-ACEE-A79976F34541}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional entry, not required</t>
         </r>
         <r>
           <rPr>
@@ -2539,7 +2470,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{0BB4A4EB-3EFC-4A5F-AA14-8C13541BE972}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{D7411B94-0C0A-415E-91F2-7398B2DD464F}">
       <text>
         <r>
           <rPr>
@@ -2563,7 +2494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{0CD8B8EB-88CD-4E7E-BC0C-513A14499F60}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A46E5A54-3492-4CC4-995C-41890EF3A9FB}">
       <text>
         <r>
           <rPr>
@@ -2587,7 +2518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{E1031546-5F91-4598-9572-207247A8A27C}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{AF8E8A0D-8218-4BE3-8F4E-F775F7661895}">
       <text>
         <r>
           <rPr>
@@ -2611,7 +2542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{4525AEAA-00B8-4B19-B136-9DB2F3D11DE7}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{39AB6324-F68A-4B7B-ADA6-8AD3F2BB0D09}">
       <text>
         <r>
           <rPr>
@@ -2635,7 +2566,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{2E058504-0E4A-4D1F-AAF5-13950C62C849}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{667BC901-3704-427A-A0DF-0ED43F631931}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{2313F2F1-29B0-465C-9B3D-C40960FC0CA1}">
       <text>
         <r>
           <rPr>
@@ -2659,7 +2614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{AC002848-4C0D-4E2B-AB44-0A1CCB8F1573}">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{3667D5C3-09C7-451C-89F9-331BBCB3A653}">
       <text>
         <r>
           <rPr>
@@ -2683,7 +2638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{0FEA709E-6C91-46BC-B25B-D9125CE43697}">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{34875AEB-942F-4EED-8EA9-1B30042F5015}">
       <text>
         <r>
           <rPr>
@@ -2694,6 +2649,102 @@
             <family val="2"/>
           </rPr>
           <t>Optional attribute data, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{0579E43D-B7E6-4954-8A5F-D03F3260A9FF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{57431432-2C56-4F07-8188-C465BAA3E506}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{9A550AEE-CC74-407E-845A-CFFF6CAEF797}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{C73CE28E-AFC3-4296-ACEE-A79976F34541}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
         </r>
         <r>
           <rPr>
@@ -2717,7 +2768,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{9D2287BD-C9AA-425F-91D5-FA688499B2B4}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{0BB4A4EB-3EFC-4A5F-AA14-8C13541BE972}">
       <text>
         <r>
           <rPr>
@@ -2741,7 +2792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{890CBB40-441E-4EF1-82C2-BE55019B15A7}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{0CD8B8EB-88CD-4E7E-BC0C-513A14499F60}">
       <text>
         <r>
           <rPr>
@@ -2765,7 +2816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{F75F94F0-3207-4492-9119-E2EE106D7165}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{E1031546-5F91-4598-9572-207247A8A27C}">
       <text>
         <r>
           <rPr>
@@ -2789,7 +2840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{169DD6B2-4ABD-447F-9D9A-61C50B1546A6}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{4525AEAA-00B8-4B19-B136-9DB2F3D11DE7}">
       <text>
         <r>
           <rPr>
@@ -2813,7 +2864,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{25355E2A-2B42-421C-B40A-594365DEA62D}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{2E058504-0E4A-4D1F-AAF5-13950C62C849}">
       <text>
         <r>
           <rPr>
@@ -2837,7 +2888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{A0012132-F763-40DB-9B7F-17773BBA2C6E}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{AC002848-4C0D-4E2B-AB44-0A1CCB8F1573}">
       <text>
         <r>
           <rPr>
@@ -2861,7 +2912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{723C11D3-B68E-4841-8CC1-B1C97832ED85}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{0FEA709E-6C91-46BC-B25B-D9125CE43697}">
       <text>
         <r>
           <rPr>
@@ -2895,7 +2946,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{735473E3-A632-4619-A928-9678F14E87AC}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{9D2287BD-C9AA-425F-91D5-FA688499B2B4}">
       <text>
         <r>
           <rPr>
@@ -2919,7 +2970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{7FF25C11-2F34-485C-9061-C0F7010551B3}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{890CBB40-441E-4EF1-82C2-BE55019B15A7}">
       <text>
         <r>
           <rPr>
@@ -2943,7 +2994,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{07D29208-3D21-4216-B66E-4744D13C0D24}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{F75F94F0-3207-4492-9119-E2EE106D7165}">
       <text>
         <r>
           <rPr>
@@ -2967,7 +3018,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{C54625A6-EE94-4A86-B1E3-D2504BE20D9F}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{169DD6B2-4ABD-447F-9D9A-61C50B1546A6}">
       <text>
         <r>
           <rPr>
@@ -2991,31 +3042,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{2E51F255-A05F-4E2F-992F-D846E20A6CB6}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attribute data, required entry</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{413E4AEA-FB83-4F07-85B3-B6F41D43BBAB}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{25355E2A-2B42-421C-B40A-594365DEA62D}">
       <text>
         <r>
           <rPr>
@@ -3039,7 +3066,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{C264D321-0534-46C5-B8F7-6EFCE58B057B}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{A0012132-F763-40DB-9B7F-17773BBA2C6E}">
       <text>
         <r>
           <rPr>
@@ -3063,7 +3090,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{35386F88-D2AA-4C63-B8A2-D24302375AD6}">
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{723C11D3-B68E-4841-8CC1-B1C97832ED85}">
       <text>
         <r>
           <rPr>
@@ -3097,7 +3124,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7B7414BA-9EB4-4752-8059-C6B5EF6E4D3E}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{735473E3-A632-4619-A928-9678F14E87AC}">
       <text>
         <r>
           <rPr>
@@ -3121,7 +3148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{165FEDD4-611C-4012-BB83-E3CE1C21FB58}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{7FF25C11-2F34-485C-9061-C0F7010551B3}">
       <text>
         <r>
           <rPr>
@@ -3145,7 +3172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{8CEB9E7A-57C6-4D28-93D7-145759F8AC8F}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{07D29208-3D21-4216-B66E-4744D13C0D24}">
       <text>
         <r>
           <rPr>
@@ -3169,7 +3196,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D9417AE5-00F5-4A5F-88BC-71AC5967C1F1}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{C54625A6-EE94-4A86-B1E3-D2504BE20D9F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{2E51F255-A05F-4E2F-992F-D846E20A6CB6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{413E4AEA-FB83-4F07-85B3-B6F41D43BBAB}">
       <text>
         <r>
           <rPr>
@@ -3193,7 +3268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{6635819A-590D-4516-B1A7-CC02EBA5D711}">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{C264D321-0534-46C5-B8F7-6EFCE58B057B}">
       <text>
         <r>
           <rPr>
@@ -3217,7 +3292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{D5BF63FF-D29C-46CA-9FCA-6D19D6D0858D}">
+    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{35386F88-D2AA-4C63-B8A2-D24302375AD6}">
       <text>
         <r>
           <rPr>
@@ -3251,7 +3326,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7EF3B599-7A3F-41D9-BC59-D5F37BC05C80}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7B7414BA-9EB4-4752-8059-C6B5EF6E4D3E}">
       <text>
         <r>
           <rPr>
@@ -3275,7 +3350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{3A1C2B96-AFA4-455B-8035-5F3A282A4566}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{165FEDD4-611C-4012-BB83-E3CE1C21FB58}">
       <text>
         <r>
           <rPr>
@@ -3299,7 +3374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{CF92F392-1B65-49DB-975A-F684212C1CC5}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{8CEB9E7A-57C6-4D28-93D7-145759F8AC8F}">
       <text>
         <r>
           <rPr>
@@ -3323,55 +3398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{40DC09A3-19F6-4D88-B9FF-A1C53673A25F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attribute data, required entry</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{499AA0DA-7765-41AC-8380-E3C3568577D8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Attribute data, required entry</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{ACFF3D53-8020-4ABF-AC94-FCC1EED66957}">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D9417AE5-00F5-4A5F-88BC-71AC5967C1F1}">
       <text>
         <r>
           <rPr>
@@ -3395,7 +3422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{4AA35DC3-5DBE-42E0-A5BE-0006736BD852}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{6635819A-590D-4516-B1A7-CC02EBA5D711}">
       <text>
         <r>
           <rPr>
@@ -3419,7 +3446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{6946CA46-9CEC-453F-B34C-D4A90132DE88}">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{D5BF63FF-D29C-46CA-9FCA-6D19D6D0858D}">
       <text>
         <r>
           <rPr>
@@ -3453,7 +3480,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{10A1CB7E-DF9D-4514-B953-8F2D062889EB}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{7EF3B599-7A3F-41D9-BC59-D5F37BC05C80}">
       <text>
         <r>
           <rPr>
@@ -3477,7 +3504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{1D7228FE-3B2F-48E5-B591-25F96F78B588}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{3A1C2B96-AFA4-455B-8035-5F3A282A4566}">
       <text>
         <r>
           <rPr>
@@ -3501,7 +3528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{5541C2EA-248D-4BD8-BA43-8C573D2A2D73}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{CF92F392-1B65-49DB-975A-F684212C1CC5}">
       <text>
         <r>
           <rPr>
@@ -3525,7 +3552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{68C59340-1672-4141-B43C-973BCCFE5B80}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{40DC09A3-19F6-4D88-B9FF-A1C53673A25F}">
       <text>
         <r>
           <rPr>
@@ -3549,7 +3576,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{A0FEDA28-9CAE-4CA1-92BC-78E062D50FA2}">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{499AA0DA-7765-41AC-8380-E3C3568577D8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{ACFF3D53-8020-4ABF-AC94-FCC1EED66957}">
       <text>
         <r>
           <rPr>
@@ -3573,7 +3624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{CA600944-93B3-4952-8879-CFB18114785B}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{4AA35DC3-5DBE-42E0-A5BE-0006736BD852}">
       <text>
         <r>
           <rPr>
@@ -3597,7 +3648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{ABF21F13-3A67-41D0-AA3F-DFDE138AB7FF}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{6946CA46-9CEC-453F-B34C-D4A90132DE88}">
       <text>
         <r>
           <rPr>
@@ -3631,7 +3682,7 @@
     <author>Odharo, Azeza L. (Assoc)</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DE34769F-A16A-413C-BC09-468D3FC8BFCF}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{10A1CB7E-DF9D-4514-B953-8F2D062889EB}">
       <text>
         <r>
           <rPr>
@@ -3655,7 +3706,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{9F26FE00-97B1-44C5-A952-04109A09EDFC}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{1D7228FE-3B2F-48E5-B591-25F96F78B588}">
       <text>
         <r>
           <rPr>
@@ -3679,31 +3730,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{4F1AF70B-FD43-409E-B571-DCA201D229CC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional entry, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{D7592426-799A-4345-9400-3CB7BA28680A}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{5541C2EA-248D-4BD8-BA43-8C573D2A2D73}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{68C59340-1672-4141-B43C-973BCCFE5B80}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{A0FEDA28-9CAE-4CA1-92BC-78E062D50FA2}">
       <text>
         <r>
           <rPr>
@@ -3727,7 +3802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{534C2DC6-3146-41B0-9203-4CE9EBF50CE6}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{CA600944-93B3-4952-8879-CFB18114785B}">
       <text>
         <r>
           <rPr>
@@ -3751,31 +3826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{CE6C6AFC-19EB-4DF7-959B-0CC5EB224E55}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional attribute data, not required</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{F34B11C0-3B17-46CE-BEA4-D0AE984EF9FD}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{ABF21F13-3A67-41D0-AA3F-DFDE138AB7FF}">
       <text>
         <r>
           <rPr>
@@ -3804,6 +3855,184 @@
 </file>
 
 <file path=xl/comments28.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Odharo, Azeza L. (Assoc)</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DE34769F-A16A-413C-BC09-468D3FC8BFCF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{9F26FE00-97B1-44C5-A952-04109A09EDFC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Attribute data, required entry</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{4F1AF70B-FD43-409E-B571-DCA201D229CC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional entry, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{D7592426-799A-4345-9400-3CB7BA28680A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional attribute data, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{534C2DC6-3146-41B0-9203-4CE9EBF50CE6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional attribute data, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{CE6C6AFC-19EB-4DF7-959B-0CC5EB224E55}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional attribute data, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{F34B11C0-3B17-46CE-BEA4-D0AE984EF9FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Optional attribute data, not required</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments29.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Odharo, Azeza L. (Assoc)</author>
@@ -5240,7 +5469,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="246">
   <si>
     <t>AT-1</t>
   </si>
@@ -5954,6 +6183,30 @@
   </si>
   <si>
     <t xml:space="preserve">? </t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>An-units</t>
+  </si>
+  <si>
+    <t>A1+A2*cos(Phi)+A3*cos^2(Phi)+A4*cos^3(Phi)+A5*cos^4(Phi)</t>
+  </si>
+  <si>
+    <t>Multiharmonic</t>
   </si>
 </sst>
 </file>
@@ -6363,6 +6616,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6381,11 +6639,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -6740,8 +6993,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A11:A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6752,10 +7005,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="20" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="55"/>
     </row>
     <row r="2" spans="1:2" s="20" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -6812,19 +7065,19 @@
       <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="52" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="25"/>
     </row>
     <row r="12" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="52" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="29"/>
     </row>
     <row r="13" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="52" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="23"/>
@@ -6893,16 +7146,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7009,12 +7262,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7130,7 +7383,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="54" t="s">
         <v>115</v>
       </c>
       <c r="B17" s="1"/>
@@ -7139,7 +7392,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="54" t="s">
         <v>116</v>
       </c>
       <c r="B18" s="1"/>
@@ -7148,7 +7401,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="54" t="s">
         <v>117</v>
       </c>
       <c r="B19" s="1"/>
@@ -7496,6 +7749,143 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D48BCB-99DB-4DA2-B11F-14BF2BE37555}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="7" width="18" customWidth="1"/>
+    <col min="8" max="9" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>242</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>241</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>240</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="I8" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{34B69E36-1006-4D41-8623-D4F81A1C700D}">
+      <formula1>"?,cis,trans,cis:right,cis:left,trans:right,trans:left"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{51F4522E-23E4-4273-8771-067B4DF4A03B}">
+      <formula1>"Multiharmonic"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{44BAAFF4-CBCA-4266-B951-D039C2C3BB00}">
+      <formula1>"A1+A2*cos(Phi)+A3*cos^2(Phi)+A4*cos^3(Phi)+A5*cos^4(Phi)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{3C73DBE5-6945-4EEB-893F-D8FDE552BF5E}">
+      <formula1>"? , kcal, kJ"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -7515,12 +7905,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -7655,7 +8045,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="54" t="s">
         <v>121</v>
       </c>
       <c r="B18" s="1"/>
@@ -7665,7 +8055,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="54" t="s">
         <v>122</v>
       </c>
       <c r="B19" s="1"/>
@@ -7675,7 +8065,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="54" t="s">
         <v>123</v>
       </c>
       <c r="B20" s="1"/>
@@ -7723,7 +8113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
@@ -7862,7 +8252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -7988,7 +8378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -8009,15 +8399,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8124,7 +8514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E701295-13E7-4A34-A798-03BF4464E0DA}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11050,7 +11440,142 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="56"/>
+    </row>
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>KeywordsList!$A$1:$A$74</xm:f>
+          </x14:formula1>
+          <xm:sqref>A6:A27</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11176,142 +11701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="19"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="53"/>
-    </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-    </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-    </row>
-    <row r="5" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>KeywordsList!$A$1:$A$74</xm:f>
-          </x14:formula1>
-          <xm:sqref>A6:A27</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11431,7 +11821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11452,12 +11842,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -11573,7 +11963,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="54" t="s">
         <v>127</v>
       </c>
       <c r="B17" s="1"/>
@@ -11582,7 +11972,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="54" t="s">
         <v>128</v>
       </c>
       <c r="B18" s="1"/>
@@ -11591,7 +11981,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="54" t="s">
         <v>115</v>
       </c>
       <c r="B19" s="1"/>
@@ -11600,7 +11990,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="54" t="s">
         <v>116</v>
       </c>
       <c r="B20" s="1"/>
@@ -11650,7 +12040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11770,7 +12160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -11898,7 +12288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
@@ -12054,7 +12444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -12159,7 +12549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -12293,7 +12683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -12409,7 +12799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -12433,16 +12823,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -12477,7 +12867,7 @@
       <c r="C6" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="53" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="15" t="s">
@@ -12550,125 +12940,6 @@
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1800-000000000000}">
       <formula1>"?, ATDL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="28"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1900-000000000000}">
-      <formula1>"?, SMILES, SMARTS, CurlySMILES, SLN, InChi"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13097,6 +13368,125 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-1900-000000000000}">
+      <formula1>"?, SMILES, SMARTS, CurlySMILES, SLN, InChi"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E1CE25-A0B8-4CC6-A1A0-17C4F6DD7775}">
   <sheetPr>
@@ -13119,32 +13509,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="1:4" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="53" t="s">
         <v>232</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="53" t="s">
         <v>233</v>
       </c>
     </row>
@@ -13303,15 +13693,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -13460,12 +13850,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -13572,7 +13962,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="54" t="s">
         <v>115</v>
       </c>
       <c r="B16" s="1"/>
@@ -13581,7 +13971,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="54" t="s">
         <v>116</v>
       </c>
       <c r="B17" s="1"/>
@@ -13590,7 +13980,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="54" t="s">
         <v>117</v>
       </c>
       <c r="B18" s="1"/>
@@ -13660,15 +14050,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
@@ -13820,17 +14210,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -13955,17 +14345,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>